<commit_message>
cleaned up debug stuff and updated the alert feature
</commit_message>
<xml_diff>
--- a/dokumentation/arbeitszeiten/Arbeitszeiten_bof31844.xlsx
+++ b/dokumentation/arbeitszeiten/Arbeitszeiten_bof31844.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Desktop\DT_WS1718_02_StarCar\dokumentation\arbeitszeiten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t>Arbeitszeit je Woche:</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Weiterentwicklung GUI</t>
+  </si>
+  <si>
+    <t>Verbleibend</t>
   </si>
 </sst>
 </file>
@@ -277,7 +280,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="44">
     <dxf>
       <font>
         <sz val="12"/>
@@ -415,6 +418,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12"/>
+        <color rgb="FF006100"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1258,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1358,7 @@
       </c>
       <c r="B9" s="7">
         <f>'Dezember 2017'!G34</f>
-        <v>3.9000000000000021</v>
+        <v>9.7666666666666693</v>
       </c>
       <c r="C9">
         <f>'Dezember 2017'!C33</f>
@@ -1372,11 +1389,20 @@
       </c>
       <c r="B12" s="7">
         <f>SUM(B7:B9)</f>
-        <v>87.316666666666606</v>
+        <v>93.183333333333266</v>
       </c>
       <c r="C12">
         <f>SUM(C7:C10)</f>
         <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="28">
+        <f>C12-B12</f>
+        <v>59.816666666666734</v>
       </c>
     </row>
   </sheetData>
@@ -2169,62 +2195,62 @@
     <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="42" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="43" priority="2" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="41" priority="4">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>WEEKDAY($A8,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2">
-    <cfRule type="expression" dxfId="40" priority="5">
+    <cfRule type="expression" dxfId="41" priority="5">
       <formula>WEEKDAY($A2,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="expression" dxfId="39" priority="6">
+    <cfRule type="expression" dxfId="40" priority="6">
       <formula>WEEKDAY($A9,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="expression" dxfId="38" priority="7">
+    <cfRule type="expression" dxfId="39" priority="7">
       <formula>WEEKDAY($A15,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="37" priority="8">
+    <cfRule type="expression" dxfId="38" priority="8">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="expression" dxfId="36" priority="9">
+    <cfRule type="expression" dxfId="37" priority="9">
       <formula>WEEKDAY($A16,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="expression" dxfId="35" priority="10">
+    <cfRule type="expression" dxfId="36" priority="10">
       <formula>WEEKDAY($A22,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="expression" dxfId="34" priority="11">
+    <cfRule type="expression" dxfId="35" priority="11">
       <formula>WEEKDAY($A23,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="expression" dxfId="33" priority="12">
+    <cfRule type="expression" dxfId="34" priority="12">
       <formula>WEEKDAY($A29,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="expression" dxfId="32" priority="13">
+    <cfRule type="expression" dxfId="33" priority="13">
       <formula>WEEKDAY($A30,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="32" priority="14">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3077,52 +3103,52 @@
     <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="30" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="31" priority="2" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>WEEKDAY($A5,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="expression" dxfId="28" priority="5">
+    <cfRule type="expression" dxfId="29" priority="5">
       <formula>WEEKDAY($A6,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="expression" dxfId="27" priority="6">
+    <cfRule type="expression" dxfId="28" priority="6">
       <formula>WEEKDAY($A12,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13">
-    <cfRule type="expression" dxfId="26" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>WEEKDAY($A13,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="expression" dxfId="25" priority="8">
+    <cfRule type="expression" dxfId="26" priority="8">
       <formula>WEEKDAY($A19,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="expression" dxfId="24" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>WEEKDAY($A20,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H26">
-    <cfRule type="expression" dxfId="23" priority="10">
+    <cfRule type="expression" dxfId="24" priority="10">
       <formula>WEEKDAY($A26,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H27">
-    <cfRule type="expression" dxfId="22" priority="11">
+    <cfRule type="expression" dxfId="23" priority="11">
       <formula>WEEKDAY($A27,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="22" priority="12">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3136,7 +3162,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3191,12 +3217,19 @@
         <f t="shared" ref="C2:C32" si="1">WEEKNUM(A2,2)</f>
         <v>49</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="24">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E2" s="24">
+        <v>0.55208333333333337</v>
+      </c>
       <c r="F2" s="24"/>
       <c r="G2" s="7">
         <f t="shared" ref="G2:G15" si="2">(E2-D2-F2)*24</f>
-        <v>0</v>
+        <v>3.2500000000000004</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -3304,12 +3337,19 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="24">
+        <v>0.8125</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.92152777777777783</v>
+      </c>
       <c r="F7" s="24"/>
       <c r="G7" s="7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.616666666666668</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3866,7 +3906,7 @@
       <c r="F34" s="38"/>
       <c r="G34" s="39">
         <f>SUM(G2:G32)</f>
-        <v>3.9000000000000021</v>
+        <v>9.7666666666666693</v>
       </c>
       <c r="H34" s="39"/>
     </row>
@@ -3877,58 +3917,63 @@
     <mergeCell ref="A34:B34"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:C32">
-    <cfRule type="timePeriod" dxfId="20" priority="2" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="21" priority="3" timePeriod="yesterday">
       <formula>FLOOR(B2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H25">
-    <cfRule type="expression" dxfId="19" priority="4">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>WEEKDAY($A25,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>WEEKDAY($A31,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="18" priority="7">
       <formula>WEEKDAY($A24,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>WEEKDAY($A18,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="15" priority="8">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>WEEKDAY($A17,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>WEEKDAY($A11,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H10">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="14" priority="11">
       <formula>WEEKDAY($A10,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="13" priority="12">
       <formula>WEEKDAY($A4,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>WEEKDAY($A3,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="expression" dxfId="10" priority="13">
+    <cfRule type="expression" dxfId="11" priority="14">
       <formula>WEEKDAY($A32,2) &gt; 5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7">
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>WEEKDAY($A7,2) &gt; 5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.15972222222222199" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
added Debug to gitignore
</commit_message>
<xml_diff>
--- a/dokumentation/arbeitszeiten/Arbeitszeiten_bof31844.xlsx
+++ b/dokumentation/arbeitszeiten/Arbeitszeiten_bof31844.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>Arbeitszeit je Woche:</t>
   </si>
@@ -139,7 +139,7 @@
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -167,6 +167,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -213,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -282,6 +288,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1364,7 +1371,7 @@
       </c>
       <c r="B9" s="7">
         <f>'Dezember 2017'!G34</f>
-        <v>55.816666666666663</v>
+        <v>62.75</v>
       </c>
       <c r="C9">
         <f>'Dezember 2017'!C33</f>
@@ -1395,7 +1402,7 @@
       </c>
       <c r="B12" s="7">
         <f>SUM(B7:B9)</f>
-        <v>139.23333333333326</v>
+        <v>146.1666666666666</v>
       </c>
       <c r="C12">
         <f>SUM(C7:C10)</f>
@@ -1408,7 +1415,7 @@
       </c>
       <c r="C14" s="28">
         <f>C12-B12</f>
-        <v>13.766666666666737</v>
+        <v>6.8333333333333997</v>
       </c>
     </row>
   </sheetData>
@@ -3165,10 +3172,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3183,7 +3190,7 @@
     <col min="8" max="1025" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -3210,7 +3217,7 @@
       </c>
       <c r="I1" s="43"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>DATE(2017,12,1)</f>
         <v>43070</v>
@@ -3231,14 +3238,14 @@
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="7">
-        <f t="shared" ref="G2:G15" si="2">(E2-D2-F2)*24</f>
+        <f t="shared" ref="G2:G16" si="2">(E2-D2-F2)*24</f>
         <v>3.2500000000000004</v>
       </c>
       <c r="H2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f t="shared" ref="A3:A32" si="3">A2+1</f>
         <v>43071</v>
@@ -3260,7 +3267,7 @@
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f t="shared" si="3"/>
         <v>43072</v>
@@ -3288,7 +3295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="3"/>
         <v>43073</v>
@@ -3309,7 +3316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="3"/>
         <v>43074</v>
@@ -3330,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="3"/>
         <v>43075</v>
@@ -3358,7 +3365,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="3"/>
         <v>43076</v>
@@ -3388,7 +3395,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="3"/>
         <v>43077</v>
@@ -3416,7 +3423,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="3"/>
         <v>43078</v>
@@ -3438,7 +3445,7 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="3"/>
         <v>43079</v>
@@ -3460,7 +3467,7 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="3"/>
         <v>43080</v>
@@ -3490,7 +3497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="3"/>
         <v>43081</v>
@@ -3520,7 +3527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="3"/>
         <v>43082</v>
@@ -3550,7 +3557,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="3"/>
         <v>43083</v>
@@ -3580,7 +3587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <f t="shared" si="3"/>
         <v>43084</v>
@@ -3593,12 +3600,23 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="27">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E16" s="27">
+        <v>0.5625</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H16" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -3678,12 +3696,19 @@
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="24">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E20" s="24">
+        <v>0.87222222222222223</v>
+      </c>
       <c r="F20" s="24"/>
       <c r="G20" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.9333333333333345</v>
+      </c>
+      <c r="H20" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3964,13 +3989,12 @@
       <c r="F34" s="38"/>
       <c r="G34" s="39">
         <f>SUM(G2:G32)</f>
-        <v>55.816666666666663</v>
+        <v>62.75</v>
       </c>
       <c r="H34" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D16:G16"/>
+  <mergeCells count="2">
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
   </mergeCells>
@@ -4035,7 +4059,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.15972222222222199" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>